<commit_message>
Created folders for input_datasets and reordered columns for IDC.
</commit_message>
<xml_diff>
--- a/input_datasets/IYS_IDC_v4_DataDictionary.xlsx
+++ b/input_datasets/IYS_IDC_v4_DataDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GitHub\IYS-Integrated-Data-Collection\input_datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1765330A-2057-4B1A-B5CA-3790F9483DA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7220608D-BD51-43D2-ADC5-DCD6F15D7E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{E7D5A010-ED65-4E6D-A254-A9C243C47EBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="184">
   <si>
     <t>Tab</t>
   </si>
@@ -78,9 +78,6 @@
     <t>length_type2</t>
   </si>
   <si>
-    <t>length_units</t>
-  </si>
-  <si>
     <t>specimen_weight</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>event_type</t>
   </si>
   <si>
-    <t>alternative_event_id</t>
-  </si>
-  <si>
     <t>event_date</t>
   </si>
   <si>
@@ -231,12 +225,6 @@
     <t>wave_height_meters</t>
   </si>
   <si>
-    <t>swell_height_meters</t>
-  </si>
-  <si>
-    <t>weather_description</t>
-  </si>
-  <si>
     <t>day_of_year</t>
   </si>
   <si>
@@ -252,15 +240,6 @@
     <t>weight_method</t>
   </si>
   <si>
-    <t>catch_volume</t>
-  </si>
-  <si>
-    <t>catch_volume_units</t>
-  </si>
-  <si>
-    <t>alternative_catch_id</t>
-  </si>
-  <si>
     <t>Cruise name. GoA2019 for datasets from 2019, IYS2020 for datasets from 2020, and IYS2022 for datasets from the 2022 Expedition.</t>
   </si>
   <si>
@@ -348,12 +327,6 @@
     <t>Wave height at time of sampling event in meters</t>
   </si>
   <si>
-    <t>Swell height at the time of sampling event in meters</t>
-  </si>
-  <si>
-    <t>Description of the weather at time of sampling event</t>
-  </si>
-  <si>
     <t>Comments provided on events related to the sampling event.</t>
   </si>
   <si>
@@ -372,51 +345,15 @@
     <t>Taxonomic rank of species_recorded</t>
   </si>
   <si>
-    <t>Taxonomic rank of verbatim_identification</t>
-  </si>
-  <si>
     <t>Lifestage of species_recorded</t>
   </si>
   <si>
-    <t>Lifestage of verbatim_identification</t>
-  </si>
-  <si>
-    <t>Common name(s) for the verbatim_identification</t>
-  </si>
-  <si>
-    <t>Person who identified the organism</t>
-  </si>
-  <si>
-    <t>Date on which organism was identified</t>
-  </si>
-  <si>
-    <t>Wet weight of species recorded in the trawl</t>
-  </si>
-  <si>
-    <t>Unit of measurement for the catch_weight of the species recorded</t>
-  </si>
-  <si>
-    <t>Method used to determine the catch_weight. Either all individuals are used to determine the weight (total), or catch_weight is extrapolated from the weight (weight estimate) or volume (volume estimate) of a (sub)sample, or this is Unknown.</t>
-  </si>
-  <si>
     <t>Total individuals caught in the trawl</t>
   </si>
   <si>
-    <t>Method used to determine the catch_count. Either all individuals are counted (Total), estimated visually, extrapolate from a weight, volume or weight/volume estimate, or unknown.</t>
-  </si>
-  <si>
-    <t>The volume of a (sub)sample taken in cubic meters</t>
-  </si>
-  <si>
-    <t>Unit of measurement for the catch_volume of the species_recorded</t>
-  </si>
-  <si>
     <t>Comments associated with the species caught</t>
   </si>
   <si>
-    <t>Unique identifier as used by the organization responsible for the trawl event at a station</t>
-  </si>
-  <si>
     <t>Life Science Identifier (LSID) of the species caught, as per the World Register of Marine Species (WoRMS)</t>
   </si>
   <si>
@@ -432,9 +369,6 @@
     <t>Net used for taxonomic analysis of bongo zooplankton data.</t>
   </si>
   <si>
-    <t>Unique identifier for a species caught with a bongo</t>
-  </si>
-  <si>
     <t>Method used to preserve organism(s)</t>
   </si>
   <si>
@@ -453,9 +387,6 @@
     <t>Size class is used for specimens which were measured in groups. In this case specimen_length means upper boundary of the size group and to calculate lower boundary of the size group 'size_class_mm' should be subtracted</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of individuals within measurement. Actual for specimen measured in groups (myctophids, squid etc). </t>
-  </si>
-  <si>
     <t>Length type used to record length of specimen</t>
   </si>
   <si>
@@ -465,9 +396,6 @@
     <t>Length type associated with the second length measurement of the specimen</t>
   </si>
   <si>
-    <t>Unit of measurement used in the specimen_length and specimen_length2</t>
-  </si>
-  <si>
     <t>Weight of the specimen</t>
   </si>
   <si>
@@ -592,6 +520,63 @@
   </si>
   <si>
     <t>Presence (yes) or absence (no) of visceral adhesion on individuals, following the protocol. Information not available for 2019 and 2020 specimen data.</t>
+  </si>
+  <si>
+    <t>Original unique identifier as used by the organization responsible for the sampling event at a station</t>
+  </si>
+  <si>
+    <t>Original unique identifier as used by the organization responsible for the trawl event at a station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method used to determine the catch_count: Total (all individuals are counted), weight estimate (count is estimated based on weight of catch), estimate (count is estimated), subsampled (catch_count includes only those individuals that were relatively whole, i.e. for gelatinous spp.), or unknown. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of individuals within specific measurement size class. The associated specimen_length is the upper size limit of the associated size_class_mm. For example, if size_class_mm = 5, and specimen_length = 65, all individuals measured (number_measured) fall in the size_range of 60 - 65 mm. </t>
+  </si>
+  <si>
+    <t>Unique digital object identifier (DOI) pointing to the metadata record for the specific data record in the IYS Data Catalogue</t>
+  </si>
+  <si>
+    <t>Taxonomic rank of taxa observed</t>
+  </si>
+  <si>
+    <t>Lifestage of taxa observed</t>
+  </si>
+  <si>
+    <t>Common name(s) for the taxa observed</t>
+  </si>
+  <si>
+    <t>Person who identified the organism or taxon.</t>
+  </si>
+  <si>
+    <t>Date on which the organism or taxon was identified</t>
+  </si>
+  <si>
+    <t>Wet weight of taxa recorded in the trawl</t>
+  </si>
+  <si>
+    <t>Unit of measurement for the catch_weight of the taxa recorded</t>
+  </si>
+  <si>
+    <t>Method used to determine the catch_weight: total (all individuals are used to determine the weight), weight estimate (total catch_weight is extrapolated from a subsampled weight), volume estimate (catch_weight is extrapolated from a subsampled volume, trace (weights that are too small to be weighed accurately), or unknown.</t>
+  </si>
+  <si>
+    <t>specimen_length_units</t>
+  </si>
+  <si>
+    <t>specimen_length2_units</t>
+  </si>
+  <si>
+    <t>Unit of measurement used in the specimen_length2</t>
+  </si>
+  <si>
+    <t>Unit of measurement used in the specimen_length</t>
+  </si>
+  <si>
+    <t>Unique identifier for a species caught with a tow</t>
+  </si>
+  <si>
+    <t>Unique identifier for an individual caught with the tow</t>
   </si>
 </sst>
 </file>
@@ -1003,11 +988,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4834FA0E-9F23-4DDE-8106-919CD43B8553}">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105:XFD108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1030,1601 +1015,1529 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>85</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>107</v>
+        <v>21</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>108</v>
+        <v>66</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>109</v>
+        <v>67</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>168</v>
+      <c r="A34" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>111</v>
+        <v>2</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="A35" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="36" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>84</v>
+        <v>3</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>112</v>
+        <v>25</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>113</v>
+        <v>23</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>165</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>117</v>
+        <v>6</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>118</v>
+        <v>26</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>125</v>
+        <v>68</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C59" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-    </row>
-    <row r="58" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C63" s="3" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>147</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>147</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>147</v>
+      </c>
+      <c r="B64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" t="s">
+        <v>178</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>147</v>
+      </c>
+      <c r="B72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>147</v>
+      </c>
+      <c r="B76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>147</v>
+      </c>
+      <c r="B78" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>147</v>
+      </c>
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>147</v>
+      </c>
+      <c r="B80" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C68" s="9" t="s">
+      <c r="C80" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>147</v>
+      </c>
+      <c r="B81" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C78" s="8" t="s">
+      <c r="C81" s="9" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
+        <v>21</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C82" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>171</v>
-      </c>
-      <c r="B83" t="s">
+      <c r="C84" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C86" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C102" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>171</v>
-      </c>
-      <c r="B84" t="s">
-        <v>4</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>171</v>
-      </c>
-      <c r="B85" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>171</v>
-      </c>
-      <c r="B86" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>171</v>
-      </c>
-      <c r="B87" t="s">
-        <v>7</v>
-      </c>
-      <c r="C87" s="9" t="s">
+    <row r="103" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>171</v>
-      </c>
-      <c r="B88" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>171</v>
-      </c>
-      <c r="B89" t="s">
-        <v>9</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>171</v>
-      </c>
-      <c r="B90" t="s">
-        <v>24</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>171</v>
-      </c>
-      <c r="B91" t="s">
-        <v>10</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>171</v>
-      </c>
-      <c r="B92" t="s">
-        <v>11</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>171</v>
-      </c>
-      <c r="B93" t="s">
-        <v>12</v>
-      </c>
-      <c r="C93" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>171</v>
-      </c>
-      <c r="B94" t="s">
-        <v>13</v>
-      </c>
-      <c r="C94" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>171</v>
-      </c>
-      <c r="B95" t="s">
-        <v>14</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>171</v>
-      </c>
-      <c r="B96" t="s">
-        <v>15</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>171</v>
-      </c>
-      <c r="B97" t="s">
-        <v>16</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>171</v>
-      </c>
-      <c r="B98" t="s">
-        <v>17</v>
-      </c>
-      <c r="C98" s="10" t="s">
+    <row r="104" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>171</v>
-      </c>
-      <c r="B99" t="s">
-        <v>18</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>171</v>
-      </c>
-      <c r="B100" t="s">
-        <v>19</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>171</v>
-      </c>
-      <c r="B101" t="s">
-        <v>20</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>171</v>
-      </c>
-      <c r="B102" t="s">
+      <c r="B104" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C102" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>171</v>
-      </c>
-      <c r="B103" t="s">
-        <v>22</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>171</v>
-      </c>
-      <c r="B104" t="s">
-        <v>23</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>152</v>
+      <c r="C104" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>171</v>
-      </c>
-      <c r="B105" t="s">
-        <v>25</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>153</v>
-      </c>
+      <c r="A105" s="3"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="9"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>171</v>
-      </c>
-      <c r="B106" t="s">
-        <v>26</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>154</v>
+        <v>148</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C106" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>171</v>
-      </c>
-      <c r="B107" t="s">
-        <v>185</v>
-      </c>
-      <c r="C107" s="9" t="s">
-        <v>186</v>
+        <v>148</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>171</v>
-      </c>
-      <c r="B108" t="s">
-        <v>187</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>188</v>
+        <v>148</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>171</v>
-      </c>
-      <c r="B109" t="s">
-        <v>27</v>
-      </c>
-      <c r="C109" s="9" t="s">
-        <v>155</v>
+        <v>148</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>148</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C111" t="s">
-        <v>78</v>
+        <v>2</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>79</v>
+        <v>24</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C113" s="5" t="s">
-        <v>80</v>
+        <v>45</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>85</v>
+        <v>49</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C118" s="8" t="s">
-        <v>86</v>
+        <v>50</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B119" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>87</v>
+        <v>51</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C120" s="5" t="s">
-        <v>88</v>
+        <v>52</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>89</v>
+        <v>53</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C129" s="9" t="s">
-        <v>97</v>
+        <v>61</v>
+      </c>
+      <c r="C129" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C134" s="11" t="s">
-        <v>102</v>
+        <v>21</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C135" s="9" t="s">
-        <v>103</v>
+        <v>66</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C136" s="9" t="s">
-        <v>104</v>
+        <v>67</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C137" s="9" t="s">
-        <v>105</v>
+        <v>149</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C138" s="9" t="s">
-        <v>106</v>
+        <v>150</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C139" s="9" t="s">
-        <v>107</v>
+        <v>151</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C140" s="9" t="s">
-        <v>108</v>
+        <v>152</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C141" s="5" t="s">
-        <v>109</v>
+        <v>153</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>172</v>
-      </c>
-      <c r="B143" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C143" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>172</v>
-      </c>
-      <c r="B144" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="C144" s="8" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>172</v>
-      </c>
-      <c r="B145" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="C145" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>172</v>
-      </c>
-      <c r="B146" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="C146" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>172</v>
-      </c>
-      <c r="B147" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="C147" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>172</v>
-      </c>
-      <c r="B148" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="C148" s="8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>172</v>
-      </c>
-      <c r="B149" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="C149" s="8" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final changes and update to changelog.
</commit_message>
<xml_diff>
--- a/input_datasets/IYS_IDC_v4_DataDictionary.xlsx
+++ b/input_datasets/IYS_IDC_v4_DataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GitHub\IYS-Integrated-Data-Collection\input_datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7220608D-BD51-43D2-ADC5-DCD6F15D7E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DF82F0-8792-4D9A-B127-46E476998A39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{E7D5A010-ED65-4E6D-A254-A9C243C47EBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="185">
   <si>
     <t>Tab</t>
   </si>
@@ -573,10 +573,13 @@
     <t>Unit of measurement used in the specimen_length</t>
   </si>
   <si>
-    <t>Unique identifier for a species caught with a tow</t>
-  </si>
-  <si>
     <t>Unique identifier for an individual caught with the tow</t>
+  </si>
+  <si>
+    <t>net_id</t>
+  </si>
+  <si>
+    <t>Unique identifier specific to the net used in the sampling event.</t>
   </si>
 </sst>
 </file>
@@ -991,8 +994,8 @@
   <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A105" sqref="A105:XFD108"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1924,10 +1927,10 @@
         <v>146</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>3</v>
+        <v>183</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="87" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1938,7 +1941,7 @@
         <v>4</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>